<commit_message>
Datos actualizados a junio 2021 (30/8/2021)
</commit_message>
<xml_diff>
--- a/Datos_a_Junio/DESEMBARQUE_agosto.xlsx
+++ b/Datos_a_Junio/DESEMBARQUE_agosto.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mariajosezunigabasualto/MJZ/CTP2022/SARDINAAUSTRAL_LAGOS/PRIMER_INFORME/Datos_a_Junio/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57B088E9-92BC-7743-9113-82D1AB57A474}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18CB4234-24CE-7F49-8352-2152FBDEF618}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="29040" windowHeight="16000" activeTab="2" xr2:uid="{D73FE552-5237-42B3-AA1B-489DDDA3A168}"/>
+    <workbookView xWindow="400" yWindow="500" windowWidth="21580" windowHeight="16000" activeTab="2" xr2:uid="{D73FE552-5237-42B3-AA1B-489DDDA3A168}"/>
   </bookViews>
   <sheets>
     <sheet name="XI Region " sheetId="2" r:id="rId1"/>
@@ -21,6 +21,16 @@
     <externalReference r:id="rId4"/>
   </externalReferences>
   <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">MES!$P$4:$P$18</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">MES!$Q$4:$Q$18</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">MES!$R$4:$R$18</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">MES!$S$4:$S$18</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">MES!$T$4:$T$18</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">MES!$P$4:$P$18</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">MES!$Q$4:$Q$18</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">MES!$R$4:$R$18</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">MES!$S$4:$S$18</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">MES!$T$4:$T$18</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">'X Region'!$B$2:$G$62</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'XI Region '!$A$22:$G$65</definedName>
   </definedNames>
@@ -43,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="39">
   <si>
     <t>Evolución de las capturas de las principales especies,</t>
   </si>
@@ -156,12 +166,27 @@
       <t>(a JULIO)</t>
     </r>
   </si>
+  <si>
+    <t>s1</t>
+  </si>
+  <si>
+    <t>s2</t>
+  </si>
+  <si>
+    <t>s3</t>
+  </si>
+  <si>
+    <t>s4</t>
+  </si>
+  <si>
+    <t>s0</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -211,6 +236,12 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -445,7 +476,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -589,6 +620,21 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2350,6 +2396,1571 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-MX"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-MX"/>
+              <a:t>Proporción de captura entre septiembre -</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="es-MX" baseline="0"/>
+              <a:t> diciembre </a:t>
+            </a:r>
+            <a:endParaRPr lang="es-MX"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-CL"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>MES!$A$4:$A$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>2006</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2007</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2008</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2009</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2011</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2019</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2020</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2021</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>MES!$P$4:$P$18</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>0.21981379550654226</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.13337089896920104</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.4008378943324119</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.6516555354968327E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.4269521472853723E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.33406635940309887</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.2939079969552421E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.22765846036014198</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.29065058853071896</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.13778150229874828</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.20850375034805702</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.25215975615450908</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.61210621180604585</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.24218130370437152</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.55759969642951002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-94C3-F049-AA4F-13D105F8A903}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>MES!$A$4:$A$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>2006</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2007</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2008</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2009</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2011</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2019</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2020</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2021</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>MES!$Q$4:$Q$19</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>0.26</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.26</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.26</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.26</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.26</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.26</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.26</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.26</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.26</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.26</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.26</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.26</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.26</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.26</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.26</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.26</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-94C3-F049-AA4F-13D105F8A903}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>MES!$A$4:$A$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>2006</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2007</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2008</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2009</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2011</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2019</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2020</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2021</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>MES!$R$4:$R$19</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>0.09</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.09</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.09</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.09</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.09</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.09</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.09</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.09</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.09</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.09</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.09</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.09</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.09</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.09</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.09</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.09</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-94C3-F049-AA4F-13D105F8A903}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>MES!$A$4:$A$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>2006</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2007</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2008</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2009</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2011</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2019</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2020</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2021</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>MES!$S$4:$S$19</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>0.42</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.42</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.42</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.42</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.42</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.42</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.42</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.42</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.42</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.42</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.42</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.42</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.42</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.42</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.42</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.42</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-94C3-F049-AA4F-13D105F8A903}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>MES!$A$4:$A$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>2006</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2007</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2008</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2009</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2011</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2019</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2020</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2021</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>MES!$U$4:$U$19</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>0.52</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.52</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.52</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.52</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.52</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.52</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.52</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.52</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.52</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.52</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.52</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.52</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.52</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.52</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.52</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.52</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-94C3-F049-AA4F-13D105F8A903}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="226120767"/>
+        <c:axId val="226472319"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="226120767"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="226472319"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="226472319"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="226120767"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-CL"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -2499,6 +4110,47 @@
         </a:p>
       </xdr:txBody>
     </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>6350</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>825500</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3E9CE1AB-AD6E-A749-AAF0-D0E7ADA8B718}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -4293,10 +5945,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1204860-D74C-4820-9105-F5F83CDB7EC9}">
-  <dimension ref="A2:AD19"/>
+  <dimension ref="A2:AI24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P40" sqref="P40"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="Q29" sqref="Q29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -4304,7 +5956,7 @@
     <col min="1" max="16384" width="11.5" style="28"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.15">
       <c r="A2" s="47" t="s">
         <v>31</v>
       </c>
@@ -4312,7 +5964,7 @@
       <c r="C2" s="47"/>
       <c r="D2" s="47"/>
     </row>
-    <row r="3" spans="1:30" ht="23.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:35" ht="23.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="34" t="s">
         <v>2</v>
       </c>
@@ -4355,14 +6007,14 @@
       <c r="N3" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="Q3" s="48" t="s">
+      <c r="V3" s="48" t="s">
         <v>32</v>
       </c>
-      <c r="R3" s="47"/>
-      <c r="S3" s="47"/>
-      <c r="T3" s="47"/>
-    </row>
-    <row r="4" spans="1:30" ht="14" x14ac:dyDescent="0.15">
+      <c r="W3" s="47"/>
+      <c r="X3" s="47"/>
+      <c r="Y3" s="47"/>
+    </row>
+    <row r="4" spans="1:35" ht="14" x14ac:dyDescent="0.15">
       <c r="A4" s="32">
         <v>2006</v>
       </c>
@@ -4404,50 +6056,73 @@
         <f>SUM(B4:M4)</f>
         <v>35959.39</v>
       </c>
-      <c r="Q4" s="34" t="s">
+      <c r="O4" s="49">
+        <f>+SUM(J4:M4)</f>
+        <v>7904.3700000000008</v>
+      </c>
+      <c r="P4" s="50">
+        <f>+O4/N4</f>
+        <v>0.21981379550654226</v>
+      </c>
+      <c r="Q4" s="50">
+        <v>0.26</v>
+      </c>
+      <c r="R4" s="50">
+        <v>0.09</v>
+      </c>
+      <c r="S4" s="50">
+        <v>0.42</v>
+      </c>
+      <c r="T4" s="50">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="U4" s="50">
+        <v>0.52</v>
+      </c>
+      <c r="V4" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="R4" s="35" t="s">
+      <c r="W4" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="S4" s="35" t="s">
+      <c r="X4" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="T4" s="35" t="s">
+      <c r="Y4" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="U4" s="35" t="s">
+      <c r="Z4" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="V4" s="35" t="s">
+      <c r="AA4" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="W4" s="35" t="s">
+      <c r="AB4" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="X4" s="35" t="s">
+      <c r="AC4" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="Y4" s="35" t="s">
+      <c r="AD4" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="Z4" s="35" t="s">
+      <c r="AE4" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="AA4" s="35" t="s">
+      <c r="AF4" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="AB4" s="35" t="s">
+      <c r="AG4" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="AC4" s="35" t="s">
+      <c r="AH4" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="AD4" s="36" t="s">
+      <c r="AI4" s="36" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:30" ht="14" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:35" ht="14" x14ac:dyDescent="0.15">
       <c r="A5" s="32">
         <v>2007</v>
       </c>
@@ -4486,38 +6161,61 @@
       </c>
       <c r="M5" s="33"/>
       <c r="N5" s="33">
-        <f t="shared" ref="N5:N19" si="0">SUM(B5:M5)</f>
+        <f t="shared" ref="N5:N17" si="0">SUM(B5:M5)</f>
         <v>44473.270000000004</v>
       </c>
-      <c r="Q5" s="37">
+      <c r="O5" s="49">
+        <f t="shared" ref="O5:O18" si="1">+SUM(J5:M5)</f>
+        <v>5931.4400000000005</v>
+      </c>
+      <c r="P5" s="50">
+        <f t="shared" ref="P5:P18" si="2">+O5/N5</f>
+        <v>0.13337089896920104</v>
+      </c>
+      <c r="Q5" s="50">
+        <v>0.26</v>
+      </c>
+      <c r="R5" s="50">
+        <v>0.09</v>
+      </c>
+      <c r="S5" s="50">
+        <v>0.42</v>
+      </c>
+      <c r="T5" s="50">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="U5" s="50">
+        <v>0.52</v>
+      </c>
+      <c r="V5" s="37">
         <v>2020</v>
       </c>
-      <c r="R5" s="33">
+      <c r="W5" s="33">
         <v>514.66999999999996</v>
       </c>
-      <c r="S5" s="33">
+      <c r="X5" s="33">
         <v>449.26</v>
       </c>
-      <c r="T5" s="33"/>
-      <c r="U5" s="33"/>
-      <c r="V5" s="33"/>
-      <c r="W5" s="33"/>
-      <c r="X5" s="33"/>
       <c r="Y5" s="33"/>
       <c r="Z5" s="33"/>
       <c r="AA5" s="33"/>
-      <c r="AB5" s="33">
+      <c r="AB5" s="33"/>
+      <c r="AC5" s="33"/>
+      <c r="AD5" s="33"/>
+      <c r="AE5" s="33"/>
+      <c r="AF5" s="33"/>
+      <c r="AG5" s="33">
         <v>426.89</v>
       </c>
-      <c r="AC5" s="33">
+      <c r="AH5" s="33">
         <v>448.03000000000003</v>
       </c>
-      <c r="AD5" s="33">
-        <f>SUM(R5:AC5)</f>
+      <c r="AI5" s="33">
+        <f>SUM(W5:AH5)</f>
         <v>1838.85</v>
       </c>
     </row>
-    <row r="6" spans="1:30" ht="14" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:35" ht="14" x14ac:dyDescent="0.15">
       <c r="A6" s="32">
         <v>2008</v>
       </c>
@@ -4559,41 +6257,64 @@
         <f t="shared" si="0"/>
         <v>45079.67</v>
       </c>
-      <c r="Q6" s="37">
+      <c r="O6" s="49">
+        <f t="shared" si="1"/>
+        <v>18069.64</v>
+      </c>
+      <c r="P6" s="50">
+        <f t="shared" si="2"/>
+        <v>0.4008378943324119</v>
+      </c>
+      <c r="Q6" s="50">
+        <v>0.26</v>
+      </c>
+      <c r="R6" s="50">
+        <v>0.09</v>
+      </c>
+      <c r="S6" s="50">
+        <v>0.42</v>
+      </c>
+      <c r="T6" s="50">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="U6" s="50">
+        <v>0.52</v>
+      </c>
+      <c r="V6" s="37">
         <v>2021</v>
       </c>
-      <c r="R6" s="33">
+      <c r="W6" s="33">
         <v>246.46</v>
       </c>
-      <c r="S6" s="33">
+      <c r="X6" s="33">
         <v>580.90899999999999</v>
       </c>
-      <c r="T6" s="33">
+      <c r="Y6" s="33">
         <v>152</v>
       </c>
-      <c r="U6" s="33">
+      <c r="Z6" s="33">
         <v>180.77</v>
       </c>
-      <c r="V6" s="33">
+      <c r="AA6" s="33">
         <v>387.97</v>
       </c>
-      <c r="W6" s="33">
+      <c r="AB6" s="33">
         <v>594.41999999999985</v>
       </c>
-      <c r="X6" s="33">
+      <c r="AC6" s="33">
         <v>242.29999999999998</v>
       </c>
-      <c r="Y6" s="33"/>
-      <c r="Z6" s="33"/>
-      <c r="AA6" s="33"/>
-      <c r="AB6" s="33"/>
-      <c r="AC6" s="33"/>
-      <c r="AD6" s="33">
-        <f>SUM(R6:AC6)</f>
+      <c r="AD6" s="33"/>
+      <c r="AE6" s="33"/>
+      <c r="AF6" s="33"/>
+      <c r="AG6" s="33"/>
+      <c r="AH6" s="33"/>
+      <c r="AI6" s="33">
+        <f>SUM(W6:AH6)</f>
         <v>2384.8290000000002</v>
       </c>
     </row>
-    <row r="7" spans="1:30" ht="14" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:35" ht="14" x14ac:dyDescent="0.15">
       <c r="A7" s="32">
         <v>2009</v>
       </c>
@@ -4633,8 +6354,31 @@
         <f t="shared" si="0"/>
         <v>49222.139999999992</v>
       </c>
-    </row>
-    <row r="8" spans="1:30" ht="14" x14ac:dyDescent="0.15">
+      <c r="O7" s="49">
+        <f t="shared" si="1"/>
+        <v>4258.53</v>
+      </c>
+      <c r="P7" s="50">
+        <f t="shared" si="2"/>
+        <v>8.6516555354968327E-2</v>
+      </c>
+      <c r="Q7" s="50">
+        <v>0.26</v>
+      </c>
+      <c r="R7" s="50">
+        <v>0.09</v>
+      </c>
+      <c r="S7" s="50">
+        <v>0.42</v>
+      </c>
+      <c r="T7" s="50">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="U7" s="50">
+        <v>0.52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:35" ht="14" x14ac:dyDescent="0.15">
       <c r="A8" s="32">
         <v>2010</v>
       </c>
@@ -4676,8 +6420,31 @@
         <f t="shared" si="0"/>
         <v>20224.14</v>
       </c>
-    </row>
-    <row r="9" spans="1:30" ht="14" x14ac:dyDescent="0.15">
+      <c r="O8" s="49">
+        <f t="shared" si="1"/>
+        <v>1906.52</v>
+      </c>
+      <c r="P8" s="50">
+        <f t="shared" si="2"/>
+        <v>9.4269521472853723E-2</v>
+      </c>
+      <c r="Q8" s="50">
+        <v>0.26</v>
+      </c>
+      <c r="R8" s="50">
+        <v>0.09</v>
+      </c>
+      <c r="S8" s="50">
+        <v>0.42</v>
+      </c>
+      <c r="T8" s="50">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="U8" s="50">
+        <v>0.52</v>
+      </c>
+    </row>
+    <row r="9" spans="1:35" ht="14" x14ac:dyDescent="0.15">
       <c r="A9" s="32">
         <v>2011</v>
       </c>
@@ -4721,8 +6488,31 @@
         <f t="shared" si="0"/>
         <v>16793.400000000001</v>
       </c>
-    </row>
-    <row r="10" spans="1:30" ht="14" x14ac:dyDescent="0.15">
+      <c r="O9" s="49">
+        <f t="shared" si="1"/>
+        <v>5610.1100000000006</v>
+      </c>
+      <c r="P9" s="50">
+        <f t="shared" si="2"/>
+        <v>0.33406635940309887</v>
+      </c>
+      <c r="Q9" s="50">
+        <v>0.26</v>
+      </c>
+      <c r="R9" s="50">
+        <v>0.09</v>
+      </c>
+      <c r="S9" s="50">
+        <v>0.42</v>
+      </c>
+      <c r="T9" s="50">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="U9" s="50">
+        <v>0.52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:35" ht="14" x14ac:dyDescent="0.15">
       <c r="A10" s="32">
         <v>2012</v>
       </c>
@@ -4760,8 +6550,31 @@
         <f t="shared" si="0"/>
         <v>19719.129999999997</v>
       </c>
-    </row>
-    <row r="11" spans="1:30" ht="14" x14ac:dyDescent="0.15">
+      <c r="O10" s="49">
+        <f t="shared" si="1"/>
+        <v>649.53000000000009</v>
+      </c>
+      <c r="P10" s="50">
+        <f t="shared" si="2"/>
+        <v>3.2939079969552421E-2</v>
+      </c>
+      <c r="Q10" s="50">
+        <v>0.26</v>
+      </c>
+      <c r="R10" s="50">
+        <v>0.09</v>
+      </c>
+      <c r="S10" s="50">
+        <v>0.42</v>
+      </c>
+      <c r="T10" s="50">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="U10" s="50">
+        <v>0.52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:35" ht="14" x14ac:dyDescent="0.15">
       <c r="A11" s="32">
         <v>2013</v>
       </c>
@@ -4805,8 +6618,31 @@
         <f t="shared" si="0"/>
         <v>21751.970000000008</v>
       </c>
-    </row>
-    <row r="12" spans="1:30" ht="14" x14ac:dyDescent="0.15">
+      <c r="O11" s="49">
+        <f t="shared" si="1"/>
+        <v>4952.0199999999995</v>
+      </c>
+      <c r="P11" s="50">
+        <f t="shared" si="2"/>
+        <v>0.22765846036014198</v>
+      </c>
+      <c r="Q11" s="50">
+        <v>0.26</v>
+      </c>
+      <c r="R11" s="50">
+        <v>0.09</v>
+      </c>
+      <c r="S11" s="50">
+        <v>0.42</v>
+      </c>
+      <c r="T11" s="50">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="U11" s="50">
+        <v>0.52</v>
+      </c>
+    </row>
+    <row r="12" spans="1:35" ht="14" x14ac:dyDescent="0.15">
       <c r="A12" s="32">
         <v>2014</v>
       </c>
@@ -4850,8 +6686,31 @@
         <f t="shared" si="0"/>
         <v>22778.760000000002</v>
       </c>
-    </row>
-    <row r="13" spans="1:30" ht="14" x14ac:dyDescent="0.15">
+      <c r="O12" s="49">
+        <f t="shared" si="1"/>
+        <v>6620.66</v>
+      </c>
+      <c r="P12" s="50">
+        <f t="shared" si="2"/>
+        <v>0.29065058853071896</v>
+      </c>
+      <c r="Q12" s="50">
+        <v>0.26</v>
+      </c>
+      <c r="R12" s="50">
+        <v>0.09</v>
+      </c>
+      <c r="S12" s="50">
+        <v>0.42</v>
+      </c>
+      <c r="T12" s="50">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="U12" s="50">
+        <v>0.52</v>
+      </c>
+    </row>
+    <row r="13" spans="1:35" ht="14" x14ac:dyDescent="0.15">
       <c r="A13" s="32">
         <v>2015</v>
       </c>
@@ -4895,8 +6754,31 @@
         <f t="shared" si="0"/>
         <v>23710.73</v>
       </c>
-    </row>
-    <row r="14" spans="1:30" ht="14" x14ac:dyDescent="0.15">
+      <c r="O13" s="49">
+        <f t="shared" si="1"/>
+        <v>3266.8999999999996</v>
+      </c>
+      <c r="P13" s="50">
+        <f t="shared" si="2"/>
+        <v>0.13778150229874828</v>
+      </c>
+      <c r="Q13" s="50">
+        <v>0.26</v>
+      </c>
+      <c r="R13" s="50">
+        <v>0.09</v>
+      </c>
+      <c r="S13" s="50">
+        <v>0.42</v>
+      </c>
+      <c r="T13" s="50">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="U13" s="50">
+        <v>0.52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:35" ht="14" x14ac:dyDescent="0.15">
       <c r="A14" s="32">
         <v>2016</v>
       </c>
@@ -4940,8 +6822,31 @@
         <f t="shared" si="0"/>
         <v>18459.62</v>
       </c>
-    </row>
-    <row r="15" spans="1:30" ht="14" x14ac:dyDescent="0.15">
+      <c r="O14" s="49">
+        <f t="shared" si="1"/>
+        <v>3848.9</v>
+      </c>
+      <c r="P14" s="50">
+        <f t="shared" si="2"/>
+        <v>0.20850375034805702</v>
+      </c>
+      <c r="Q14" s="50">
+        <v>0.26</v>
+      </c>
+      <c r="R14" s="50">
+        <v>0.09</v>
+      </c>
+      <c r="S14" s="50">
+        <v>0.42</v>
+      </c>
+      <c r="T14" s="50">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="U14" s="50">
+        <v>0.52</v>
+      </c>
+    </row>
+    <row r="15" spans="1:35" ht="14" x14ac:dyDescent="0.15">
       <c r="A15" s="32">
         <v>2017</v>
       </c>
@@ -4985,8 +6890,31 @@
         <f t="shared" si="0"/>
         <v>14133.539999999999</v>
       </c>
-    </row>
-    <row r="16" spans="1:30" ht="14" x14ac:dyDescent="0.15">
+      <c r="O15" s="49">
+        <f t="shared" si="1"/>
+        <v>3563.91</v>
+      </c>
+      <c r="P15" s="50">
+        <f t="shared" si="2"/>
+        <v>0.25215975615450908</v>
+      </c>
+      <c r="Q15" s="50">
+        <v>0.26</v>
+      </c>
+      <c r="R15" s="50">
+        <v>0.09</v>
+      </c>
+      <c r="S15" s="50">
+        <v>0.42</v>
+      </c>
+      <c r="T15" s="50">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="U15" s="50">
+        <v>0.52</v>
+      </c>
+    </row>
+    <row r="16" spans="1:35" ht="14" x14ac:dyDescent="0.15">
       <c r="A16" s="32">
         <v>2018</v>
       </c>
@@ -5030,8 +6958,31 @@
         <f t="shared" si="0"/>
         <v>8355.3799999999992</v>
       </c>
-    </row>
-    <row r="17" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+      <c r="O16" s="49">
+        <f t="shared" si="1"/>
+        <v>5114.3799999999992</v>
+      </c>
+      <c r="P16" s="50">
+        <f t="shared" si="2"/>
+        <v>0.61210621180604585</v>
+      </c>
+      <c r="Q16" s="50">
+        <v>0.26</v>
+      </c>
+      <c r="R16" s="50">
+        <v>0.09</v>
+      </c>
+      <c r="S16" s="50">
+        <v>0.42</v>
+      </c>
+      <c r="T16" s="50">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="U16" s="50">
+        <v>0.52</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" ht="14" x14ac:dyDescent="0.15">
       <c r="A17" s="32">
         <v>2019</v>
       </c>
@@ -5075,8 +7026,31 @@
         <f t="shared" si="0"/>
         <v>11269.334000000001</v>
       </c>
-    </row>
-    <row r="18" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+      <c r="O17" s="49">
+        <f t="shared" si="1"/>
+        <v>2729.2220000000002</v>
+      </c>
+      <c r="P17" s="50">
+        <f t="shared" si="2"/>
+        <v>0.24218130370437152</v>
+      </c>
+      <c r="Q17" s="50">
+        <v>0.26</v>
+      </c>
+      <c r="R17" s="50">
+        <v>0.09</v>
+      </c>
+      <c r="S17" s="50">
+        <v>0.42</v>
+      </c>
+      <c r="T17" s="50">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="U17" s="50">
+        <v>0.52</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" ht="14" x14ac:dyDescent="0.15">
       <c r="A18" s="32">
         <v>2020</v>
       </c>
@@ -5120,8 +7094,31 @@
         <f>SUM(B18:M18)</f>
         <v>14193.737999999998</v>
       </c>
-    </row>
-    <row r="19" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+      <c r="O18" s="49">
+        <f t="shared" si="1"/>
+        <v>7914.4239999999991</v>
+      </c>
+      <c r="P18" s="50">
+        <f t="shared" si="2"/>
+        <v>0.55759969642951002</v>
+      </c>
+      <c r="Q18" s="50">
+        <v>0.26</v>
+      </c>
+      <c r="R18" s="50">
+        <v>0.09</v>
+      </c>
+      <c r="S18" s="50">
+        <v>0.42</v>
+      </c>
+      <c r="T18" s="50">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="U18" s="50">
+        <v>0.52</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" ht="14" x14ac:dyDescent="0.15">
       <c r="A19" s="32">
         <v>2021</v>
       </c>
@@ -5154,18 +7151,120 @@
       <c r="L19" s="33"/>
       <c r="M19" s="33"/>
       <c r="N19" s="33">
-        <f t="shared" si="0"/>
-        <v>7505.4120000000003</v>
+        <v>15765</v>
+      </c>
+      <c r="P19" s="50">
+        <f t="shared" ref="P19" si="3">+O19/N19</f>
+        <v>0</v>
+      </c>
+      <c r="Q19" s="50">
+        <v>0.26</v>
+      </c>
+      <c r="R19" s="50">
+        <v>0.09</v>
+      </c>
+      <c r="S19" s="50">
+        <v>0.42</v>
+      </c>
+      <c r="T19" s="50">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="U19" s="50">
+        <v>0.52</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="O20" s="51">
+        <f>+N19*Q4</f>
+        <v>4098.9000000000005</v>
+      </c>
+      <c r="P20" s="52">
+        <f>+SUM($B$19:$I$19)+O20</f>
+        <v>11604.312000000002</v>
+      </c>
+      <c r="R20" s="53" t="s">
+        <v>34</v>
+      </c>
+      <c r="T20" s="50"/>
+      <c r="U20" s="50"/>
+      <c r="V20" s="28">
+        <f>+STDEV(P4:P18)</f>
+        <v>0.16567315590631818</v>
+      </c>
+      <c r="W20" s="50">
+        <f>+S21+V20</f>
+        <v>0.42103684754903359</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="O21" s="51">
+        <f>+N19*R4</f>
+        <v>1418.85</v>
+      </c>
+      <c r="P21" s="52">
+        <f>+SUM($B$19:$I$19)+O21</f>
+        <v>8924.2620000000006</v>
+      </c>
+      <c r="R21" s="53" t="s">
+        <v>35</v>
+      </c>
+      <c r="S21" s="50">
+        <f>+AVERAGE(P4:P18)</f>
+        <v>0.25536369164271538</v>
+      </c>
+      <c r="W21" s="50">
+        <f>+S21-V20</f>
+        <v>8.9690535736397209E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="O22" s="51">
+        <f>+N19*S4</f>
+        <v>6621.3</v>
+      </c>
+      <c r="P22" s="52">
+        <f t="shared" ref="P22:P23" si="4">+SUM($B$19:$I$19)+O22</f>
+        <v>14126.712</v>
+      </c>
+      <c r="R22" s="53" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="O23" s="51">
+        <f>+N19*P18</f>
+        <v>8790.5592142112255</v>
+      </c>
+      <c r="P23" s="52">
+        <f t="shared" si="4"/>
+        <v>16295.971214211226</v>
+      </c>
+      <c r="R23" s="53" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="O24" s="49">
+        <f>+N19-SUM(B19:I19)</f>
+        <v>8259.5879999999997</v>
+      </c>
+      <c r="P24" s="52">
+        <f>+SUM($B$19:$I$19)+O24</f>
+        <v>15765</v>
+      </c>
+      <c r="R24" s="53" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A2:D2"/>
-    <mergeCell ref="Q3:T3"/>
+    <mergeCell ref="V3:Y3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="N4:N18 N19 AD5:AD6" formulaRange="1"/>
+    <ignoredError sqref="N4:N18 AI5:AI6" formulaRange="1"/>
   </ignoredErrors>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Datos actualizados a junio 2021 (1/09/2021)
</commit_message>
<xml_diff>
--- a/Datos_a_Junio/DESEMBARQUE_agosto.xlsx
+++ b/Datos_a_Junio/DESEMBARQUE_agosto.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mariajosezunigabasualto/MJZ/CTP2022/SARDINAAUSTRAL_LAGOS/PRIMER_INFORME/Datos_a_Junio/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18CB4234-24CE-7F49-8352-2152FBDEF618}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{953DA985-5101-1642-A060-17B62D205314}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="400" yWindow="500" windowWidth="21580" windowHeight="16000" activeTab="2" xr2:uid="{D73FE552-5237-42B3-AA1B-489DDDA3A168}"/>
+    <workbookView xWindow="27560" yWindow="3580" windowWidth="23300" windowHeight="22440" activeTab="2" xr2:uid="{D73FE552-5237-42B3-AA1B-489DDDA3A168}"/>
   </bookViews>
   <sheets>
     <sheet name="XI Region " sheetId="2" r:id="rId1"/>
@@ -21,16 +21,6 @@
     <externalReference r:id="rId4"/>
   </externalReferences>
   <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">MES!$P$4:$P$18</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">MES!$Q$4:$Q$18</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">MES!$R$4:$R$18</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">MES!$S$4:$S$18</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">MES!$T$4:$T$18</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">MES!$P$4:$P$18</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">MES!$Q$4:$Q$18</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">MES!$R$4:$R$18</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">MES!$S$4:$S$18</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">MES!$T$4:$T$18</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">'X Region'!$B$2:$G$62</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'XI Region '!$A$22:$G$65</definedName>
   </definedNames>
@@ -601,6 +591,21 @@
     <xf numFmtId="3" fontId="2" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -620,21 +625,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -4673,24 +4663,24 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="42"/>
-      <c r="G2" s="42"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="47"/>
     </row>
     <row r="3" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B3" s="43" t="s">
+      <c r="B3" s="48" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="42"/>
-      <c r="D3" s="42"/>
-      <c r="E3" s="42"/>
-      <c r="F3" s="42"/>
-      <c r="G3" s="42"/>
+      <c r="C3" s="47"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="47"/>
+      <c r="G3" s="47"/>
     </row>
     <row r="5" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" s="6" t="s">
@@ -5062,14 +5052,14 @@
       </c>
     </row>
     <row r="44" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B44" s="44" t="s">
+      <c r="B44" s="49" t="s">
         <v>13</v>
       </c>
-      <c r="C44" s="44"/>
-      <c r="D44" s="44"/>
-      <c r="E44" s="44"/>
-      <c r="F44" s="44"/>
-      <c r="G44" s="44"/>
+      <c r="C44" s="49"/>
+      <c r="D44" s="49"/>
+      <c r="E44" s="49"/>
+      <c r="F44" s="49"/>
+      <c r="G44" s="49"/>
     </row>
     <row r="66" spans="2:2" s="2" customFormat="1" ht="8.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B66" s="25"/>
@@ -5121,14 +5111,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="42"/>
-      <c r="G2" s="42"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="47"/>
       <c r="H2" s="1"/>
       <c r="J2" s="3" t="s">
         <v>1</v>
@@ -5139,14 +5129,14 @@
       <c r="N2" s="3"/>
     </row>
     <row r="3" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B3" s="43" t="s">
+      <c r="B3" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="42"/>
-      <c r="D3" s="42"/>
-      <c r="E3" s="42"/>
-      <c r="F3" s="42"/>
-      <c r="G3" s="42"/>
+      <c r="C3" s="47"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="47"/>
+      <c r="G3" s="47"/>
       <c r="H3" s="1"/>
     </row>
     <row r="5" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.15">
@@ -5890,14 +5880,14 @@
       <c r="Q45" s="31"/>
     </row>
     <row r="46" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A46" s="45" t="s">
+      <c r="A46" s="50" t="s">
         <v>14</v>
       </c>
-      <c r="B46" s="46"/>
-      <c r="C46" s="46"/>
-      <c r="D46" s="46"/>
-      <c r="E46" s="46"/>
-      <c r="F46" s="46"/>
+      <c r="B46" s="51"/>
+      <c r="C46" s="51"/>
+      <c r="D46" s="51"/>
+      <c r="E46" s="51"/>
+      <c r="F46" s="51"/>
       <c r="K46" s="31"/>
       <c r="L46" s="31"/>
       <c r="M46" s="31"/>
@@ -5947,7 +5937,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1204860-D74C-4820-9105-F5F83CDB7EC9}">
   <dimension ref="A2:AI24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="Q29" sqref="Q29"/>
     </sheetView>
   </sheetViews>
@@ -5957,12 +5947,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:35" x14ac:dyDescent="0.15">
-      <c r="A2" s="47" t="s">
+      <c r="A2" s="52" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="47"/>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
+      <c r="B2" s="52"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
     </row>
     <row r="3" spans="1:35" ht="23.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="34" t="s">
@@ -6007,12 +5997,12 @@
       <c r="N3" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="V3" s="48" t="s">
+      <c r="V3" s="53" t="s">
         <v>32</v>
       </c>
-      <c r="W3" s="47"/>
-      <c r="X3" s="47"/>
-      <c r="Y3" s="47"/>
+      <c r="W3" s="52"/>
+      <c r="X3" s="52"/>
+      <c r="Y3" s="52"/>
     </row>
     <row r="4" spans="1:35" ht="14" x14ac:dyDescent="0.15">
       <c r="A4" s="32">
@@ -6056,27 +6046,27 @@
         <f>SUM(B4:M4)</f>
         <v>35959.39</v>
       </c>
-      <c r="O4" s="49">
+      <c r="O4" s="42">
         <f>+SUM(J4:M4)</f>
         <v>7904.3700000000008</v>
       </c>
-      <c r="P4" s="50">
+      <c r="P4" s="43">
         <f>+O4/N4</f>
         <v>0.21981379550654226</v>
       </c>
-      <c r="Q4" s="50">
+      <c r="Q4" s="43">
         <v>0.26</v>
       </c>
-      <c r="R4" s="50">
+      <c r="R4" s="43">
         <v>0.09</v>
       </c>
-      <c r="S4" s="50">
+      <c r="S4" s="43">
         <v>0.42</v>
       </c>
-      <c r="T4" s="50">
+      <c r="T4" s="43">
         <v>0.56000000000000005</v>
       </c>
-      <c r="U4" s="50">
+      <c r="U4" s="43">
         <v>0.52</v>
       </c>
       <c r="V4" s="34" t="s">
@@ -6164,27 +6154,27 @@
         <f t="shared" ref="N5:N17" si="0">SUM(B5:M5)</f>
         <v>44473.270000000004</v>
       </c>
-      <c r="O5" s="49">
+      <c r="O5" s="42">
         <f t="shared" ref="O5:O18" si="1">+SUM(J5:M5)</f>
         <v>5931.4400000000005</v>
       </c>
-      <c r="P5" s="50">
+      <c r="P5" s="43">
         <f t="shared" ref="P5:P18" si="2">+O5/N5</f>
         <v>0.13337089896920104</v>
       </c>
-      <c r="Q5" s="50">
+      <c r="Q5" s="43">
         <v>0.26</v>
       </c>
-      <c r="R5" s="50">
+      <c r="R5" s="43">
         <v>0.09</v>
       </c>
-      <c r="S5" s="50">
+      <c r="S5" s="43">
         <v>0.42</v>
       </c>
-      <c r="T5" s="50">
+      <c r="T5" s="43">
         <v>0.56000000000000005</v>
       </c>
-      <c r="U5" s="50">
+      <c r="U5" s="43">
         <v>0.52</v>
       </c>
       <c r="V5" s="37">
@@ -6257,27 +6247,27 @@
         <f t="shared" si="0"/>
         <v>45079.67</v>
       </c>
-      <c r="O6" s="49">
+      <c r="O6" s="42">
         <f t="shared" si="1"/>
         <v>18069.64</v>
       </c>
-      <c r="P6" s="50">
+      <c r="P6" s="43">
         <f t="shared" si="2"/>
         <v>0.4008378943324119</v>
       </c>
-      <c r="Q6" s="50">
+      <c r="Q6" s="43">
         <v>0.26</v>
       </c>
-      <c r="R6" s="50">
+      <c r="R6" s="43">
         <v>0.09</v>
       </c>
-      <c r="S6" s="50">
+      <c r="S6" s="43">
         <v>0.42</v>
       </c>
-      <c r="T6" s="50">
+      <c r="T6" s="43">
         <v>0.56000000000000005</v>
       </c>
-      <c r="U6" s="50">
+      <c r="U6" s="43">
         <v>0.52</v>
       </c>
       <c r="V6" s="37">
@@ -6354,27 +6344,27 @@
         <f t="shared" si="0"/>
         <v>49222.139999999992</v>
       </c>
-      <c r="O7" s="49">
+      <c r="O7" s="42">
         <f t="shared" si="1"/>
         <v>4258.53</v>
       </c>
-      <c r="P7" s="50">
+      <c r="P7" s="43">
         <f t="shared" si="2"/>
         <v>8.6516555354968327E-2</v>
       </c>
-      <c r="Q7" s="50">
+      <c r="Q7" s="43">
         <v>0.26</v>
       </c>
-      <c r="R7" s="50">
+      <c r="R7" s="43">
         <v>0.09</v>
       </c>
-      <c r="S7" s="50">
+      <c r="S7" s="43">
         <v>0.42</v>
       </c>
-      <c r="T7" s="50">
+      <c r="T7" s="43">
         <v>0.56000000000000005</v>
       </c>
-      <c r="U7" s="50">
+      <c r="U7" s="43">
         <v>0.52</v>
       </c>
     </row>
@@ -6420,27 +6410,27 @@
         <f t="shared" si="0"/>
         <v>20224.14</v>
       </c>
-      <c r="O8" s="49">
+      <c r="O8" s="42">
         <f t="shared" si="1"/>
         <v>1906.52</v>
       </c>
-      <c r="P8" s="50">
+      <c r="P8" s="43">
         <f t="shared" si="2"/>
         <v>9.4269521472853723E-2</v>
       </c>
-      <c r="Q8" s="50">
+      <c r="Q8" s="43">
         <v>0.26</v>
       </c>
-      <c r="R8" s="50">
+      <c r="R8" s="43">
         <v>0.09</v>
       </c>
-      <c r="S8" s="50">
+      <c r="S8" s="43">
         <v>0.42</v>
       </c>
-      <c r="T8" s="50">
+      <c r="T8" s="43">
         <v>0.56000000000000005</v>
       </c>
-      <c r="U8" s="50">
+      <c r="U8" s="43">
         <v>0.52</v>
       </c>
     </row>
@@ -6488,27 +6478,27 @@
         <f t="shared" si="0"/>
         <v>16793.400000000001</v>
       </c>
-      <c r="O9" s="49">
+      <c r="O9" s="42">
         <f t="shared" si="1"/>
         <v>5610.1100000000006</v>
       </c>
-      <c r="P9" s="50">
+      <c r="P9" s="43">
         <f t="shared" si="2"/>
         <v>0.33406635940309887</v>
       </c>
-      <c r="Q9" s="50">
+      <c r="Q9" s="43">
         <v>0.26</v>
       </c>
-      <c r="R9" s="50">
+      <c r="R9" s="43">
         <v>0.09</v>
       </c>
-      <c r="S9" s="50">
+      <c r="S9" s="43">
         <v>0.42</v>
       </c>
-      <c r="T9" s="50">
+      <c r="T9" s="43">
         <v>0.56000000000000005</v>
       </c>
-      <c r="U9" s="50">
+      <c r="U9" s="43">
         <v>0.52</v>
       </c>
     </row>
@@ -6550,27 +6540,27 @@
         <f t="shared" si="0"/>
         <v>19719.129999999997</v>
       </c>
-      <c r="O10" s="49">
+      <c r="O10" s="42">
         <f t="shared" si="1"/>
         <v>649.53000000000009</v>
       </c>
-      <c r="P10" s="50">
+      <c r="P10" s="43">
         <f t="shared" si="2"/>
         <v>3.2939079969552421E-2</v>
       </c>
-      <c r="Q10" s="50">
+      <c r="Q10" s="43">
         <v>0.26</v>
       </c>
-      <c r="R10" s="50">
+      <c r="R10" s="43">
         <v>0.09</v>
       </c>
-      <c r="S10" s="50">
+      <c r="S10" s="43">
         <v>0.42</v>
       </c>
-      <c r="T10" s="50">
+      <c r="T10" s="43">
         <v>0.56000000000000005</v>
       </c>
-      <c r="U10" s="50">
+      <c r="U10" s="43">
         <v>0.52</v>
       </c>
     </row>
@@ -6618,27 +6608,27 @@
         <f t="shared" si="0"/>
         <v>21751.970000000008</v>
       </c>
-      <c r="O11" s="49">
+      <c r="O11" s="42">
         <f t="shared" si="1"/>
         <v>4952.0199999999995</v>
       </c>
-      <c r="P11" s="50">
+      <c r="P11" s="43">
         <f t="shared" si="2"/>
         <v>0.22765846036014198</v>
       </c>
-      <c r="Q11" s="50">
+      <c r="Q11" s="43">
         <v>0.26</v>
       </c>
-      <c r="R11" s="50">
+      <c r="R11" s="43">
         <v>0.09</v>
       </c>
-      <c r="S11" s="50">
+      <c r="S11" s="43">
         <v>0.42</v>
       </c>
-      <c r="T11" s="50">
+      <c r="T11" s="43">
         <v>0.56000000000000005</v>
       </c>
-      <c r="U11" s="50">
+      <c r="U11" s="43">
         <v>0.52</v>
       </c>
     </row>
@@ -6686,27 +6676,27 @@
         <f t="shared" si="0"/>
         <v>22778.760000000002</v>
       </c>
-      <c r="O12" s="49">
+      <c r="O12" s="42">
         <f t="shared" si="1"/>
         <v>6620.66</v>
       </c>
-      <c r="P12" s="50">
+      <c r="P12" s="43">
         <f t="shared" si="2"/>
         <v>0.29065058853071896</v>
       </c>
-      <c r="Q12" s="50">
+      <c r="Q12" s="43">
         <v>0.26</v>
       </c>
-      <c r="R12" s="50">
+      <c r="R12" s="43">
         <v>0.09</v>
       </c>
-      <c r="S12" s="50">
+      <c r="S12" s="43">
         <v>0.42</v>
       </c>
-      <c r="T12" s="50">
+      <c r="T12" s="43">
         <v>0.56000000000000005</v>
       </c>
-      <c r="U12" s="50">
+      <c r="U12" s="43">
         <v>0.52</v>
       </c>
     </row>
@@ -6754,27 +6744,27 @@
         <f t="shared" si="0"/>
         <v>23710.73</v>
       </c>
-      <c r="O13" s="49">
+      <c r="O13" s="42">
         <f t="shared" si="1"/>
         <v>3266.8999999999996</v>
       </c>
-      <c r="P13" s="50">
+      <c r="P13" s="43">
         <f t="shared" si="2"/>
         <v>0.13778150229874828</v>
       </c>
-      <c r="Q13" s="50">
+      <c r="Q13" s="43">
         <v>0.26</v>
       </c>
-      <c r="R13" s="50">
+      <c r="R13" s="43">
         <v>0.09</v>
       </c>
-      <c r="S13" s="50">
+      <c r="S13" s="43">
         <v>0.42</v>
       </c>
-      <c r="T13" s="50">
+      <c r="T13" s="43">
         <v>0.56000000000000005</v>
       </c>
-      <c r="U13" s="50">
+      <c r="U13" s="43">
         <v>0.52</v>
       </c>
     </row>
@@ -6822,27 +6812,27 @@
         <f t="shared" si="0"/>
         <v>18459.62</v>
       </c>
-      <c r="O14" s="49">
+      <c r="O14" s="42">
         <f t="shared" si="1"/>
         <v>3848.9</v>
       </c>
-      <c r="P14" s="50">
+      <c r="P14" s="43">
         <f t="shared" si="2"/>
         <v>0.20850375034805702</v>
       </c>
-      <c r="Q14" s="50">
+      <c r="Q14" s="43">
         <v>0.26</v>
       </c>
-      <c r="R14" s="50">
+      <c r="R14" s="43">
         <v>0.09</v>
       </c>
-      <c r="S14" s="50">
+      <c r="S14" s="43">
         <v>0.42</v>
       </c>
-      <c r="T14" s="50">
+      <c r="T14" s="43">
         <v>0.56000000000000005</v>
       </c>
-      <c r="U14" s="50">
+      <c r="U14" s="43">
         <v>0.52</v>
       </c>
     </row>
@@ -6890,27 +6880,27 @@
         <f t="shared" si="0"/>
         <v>14133.539999999999</v>
       </c>
-      <c r="O15" s="49">
+      <c r="O15" s="42">
         <f t="shared" si="1"/>
         <v>3563.91</v>
       </c>
-      <c r="P15" s="50">
+      <c r="P15" s="43">
         <f t="shared" si="2"/>
         <v>0.25215975615450908</v>
       </c>
-      <c r="Q15" s="50">
+      <c r="Q15" s="43">
         <v>0.26</v>
       </c>
-      <c r="R15" s="50">
+      <c r="R15" s="43">
         <v>0.09</v>
       </c>
-      <c r="S15" s="50">
+      <c r="S15" s="43">
         <v>0.42</v>
       </c>
-      <c r="T15" s="50">
+      <c r="T15" s="43">
         <v>0.56000000000000005</v>
       </c>
-      <c r="U15" s="50">
+      <c r="U15" s="43">
         <v>0.52</v>
       </c>
     </row>
@@ -6958,27 +6948,27 @@
         <f t="shared" si="0"/>
         <v>8355.3799999999992</v>
       </c>
-      <c r="O16" s="49">
+      <c r="O16" s="42">
         <f t="shared" si="1"/>
         <v>5114.3799999999992</v>
       </c>
-      <c r="P16" s="50">
+      <c r="P16" s="43">
         <f t="shared" si="2"/>
         <v>0.61210621180604585</v>
       </c>
-      <c r="Q16" s="50">
+      <c r="Q16" s="43">
         <v>0.26</v>
       </c>
-      <c r="R16" s="50">
+      <c r="R16" s="43">
         <v>0.09</v>
       </c>
-      <c r="S16" s="50">
+      <c r="S16" s="43">
         <v>0.42</v>
       </c>
-      <c r="T16" s="50">
+      <c r="T16" s="43">
         <v>0.56000000000000005</v>
       </c>
-      <c r="U16" s="50">
+      <c r="U16" s="43">
         <v>0.52</v>
       </c>
     </row>
@@ -7026,27 +7016,27 @@
         <f t="shared" si="0"/>
         <v>11269.334000000001</v>
       </c>
-      <c r="O17" s="49">
+      <c r="O17" s="42">
         <f t="shared" si="1"/>
         <v>2729.2220000000002</v>
       </c>
-      <c r="P17" s="50">
+      <c r="P17" s="43">
         <f t="shared" si="2"/>
         <v>0.24218130370437152</v>
       </c>
-      <c r="Q17" s="50">
+      <c r="Q17" s="43">
         <v>0.26</v>
       </c>
-      <c r="R17" s="50">
+      <c r="R17" s="43">
         <v>0.09</v>
       </c>
-      <c r="S17" s="50">
+      <c r="S17" s="43">
         <v>0.42</v>
       </c>
-      <c r="T17" s="50">
+      <c r="T17" s="43">
         <v>0.56000000000000005</v>
       </c>
-      <c r="U17" s="50">
+      <c r="U17" s="43">
         <v>0.52</v>
       </c>
     </row>
@@ -7094,27 +7084,27 @@
         <f>SUM(B18:M18)</f>
         <v>14193.737999999998</v>
       </c>
-      <c r="O18" s="49">
+      <c r="O18" s="42">
         <f t="shared" si="1"/>
         <v>7914.4239999999991</v>
       </c>
-      <c r="P18" s="50">
+      <c r="P18" s="43">
         <f t="shared" si="2"/>
         <v>0.55759969642951002</v>
       </c>
-      <c r="Q18" s="50">
+      <c r="Q18" s="43">
         <v>0.26</v>
       </c>
-      <c r="R18" s="50">
+      <c r="R18" s="43">
         <v>0.09</v>
       </c>
-      <c r="S18" s="50">
+      <c r="S18" s="43">
         <v>0.42</v>
       </c>
-      <c r="T18" s="50">
+      <c r="T18" s="43">
         <v>0.56000000000000005</v>
       </c>
-      <c r="U18" s="50">
+      <c r="U18" s="43">
         <v>0.52</v>
       </c>
     </row>
@@ -7153,106 +7143,106 @@
       <c r="N19" s="33">
         <v>15765</v>
       </c>
-      <c r="P19" s="50">
+      <c r="P19" s="43">
         <f t="shared" ref="P19" si="3">+O19/N19</f>
         <v>0</v>
       </c>
-      <c r="Q19" s="50">
+      <c r="Q19" s="43">
         <v>0.26</v>
       </c>
-      <c r="R19" s="50">
+      <c r="R19" s="43">
         <v>0.09</v>
       </c>
-      <c r="S19" s="50">
+      <c r="S19" s="43">
         <v>0.42</v>
       </c>
-      <c r="T19" s="50">
+      <c r="T19" s="43">
         <v>0.56000000000000005</v>
       </c>
-      <c r="U19" s="50">
+      <c r="U19" s="43">
         <v>0.52</v>
       </c>
     </row>
     <row r="20" spans="1:23" x14ac:dyDescent="0.15">
-      <c r="O20" s="51">
+      <c r="O20" s="44">
         <f>+N19*Q4</f>
         <v>4098.9000000000005</v>
       </c>
-      <c r="P20" s="52">
+      <c r="P20" s="45">
         <f>+SUM($B$19:$I$19)+O20</f>
         <v>11604.312000000002</v>
       </c>
-      <c r="R20" s="53" t="s">
+      <c r="R20" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="T20" s="50"/>
-      <c r="U20" s="50"/>
+      <c r="T20" s="43"/>
+      <c r="U20" s="43"/>
       <c r="V20" s="28">
         <f>+STDEV(P4:P18)</f>
         <v>0.16567315590631818</v>
       </c>
-      <c r="W20" s="50">
+      <c r="W20" s="43">
         <f>+S21+V20</f>
         <v>0.42103684754903359</v>
       </c>
     </row>
     <row r="21" spans="1:23" x14ac:dyDescent="0.15">
-      <c r="O21" s="51">
+      <c r="O21" s="44">
         <f>+N19*R4</f>
         <v>1418.85</v>
       </c>
-      <c r="P21" s="52">
+      <c r="P21" s="45">
         <f>+SUM($B$19:$I$19)+O21</f>
         <v>8924.2620000000006</v>
       </c>
-      <c r="R21" s="53" t="s">
+      <c r="R21" s="46" t="s">
         <v>35</v>
       </c>
-      <c r="S21" s="50">
+      <c r="S21" s="43">
         <f>+AVERAGE(P4:P18)</f>
         <v>0.25536369164271538</v>
       </c>
-      <c r="W21" s="50">
+      <c r="W21" s="43">
         <f>+S21-V20</f>
         <v>8.9690535736397209E-2</v>
       </c>
     </row>
     <row r="22" spans="1:23" x14ac:dyDescent="0.15">
-      <c r="O22" s="51">
+      <c r="O22" s="44">
         <f>+N19*S4</f>
         <v>6621.3</v>
       </c>
-      <c r="P22" s="52">
+      <c r="P22" s="45">
         <f t="shared" ref="P22:P23" si="4">+SUM($B$19:$I$19)+O22</f>
         <v>14126.712</v>
       </c>
-      <c r="R22" s="53" t="s">
+      <c r="R22" s="46" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="23" spans="1:23" x14ac:dyDescent="0.15">
-      <c r="O23" s="51">
+      <c r="O23" s="44">
         <f>+N19*P18</f>
         <v>8790.5592142112255</v>
       </c>
-      <c r="P23" s="52">
+      <c r="P23" s="45">
         <f t="shared" si="4"/>
         <v>16295.971214211226</v>
       </c>
-      <c r="R23" s="53" t="s">
+      <c r="R23" s="46" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="24" spans="1:23" x14ac:dyDescent="0.15">
-      <c r="O24" s="49">
+      <c r="O24" s="42">
         <f>+N19-SUM(B19:I19)</f>
         <v>8259.5879999999997</v>
       </c>
-      <c r="P24" s="52">
+      <c r="P24" s="45">
         <f>+SUM($B$19:$I$19)+O24</f>
         <v>15765</v>
       </c>
-      <c r="R24" s="53" t="s">
+      <c r="R24" s="46" t="s">
         <v>38</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Datos a junio OK 14/9/2021
</commit_message>
<xml_diff>
--- a/Datos_a_Junio/DESEMBARQUE_agosto.xlsx
+++ b/Datos_a_Junio/DESEMBARQUE_agosto.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mariajosezunigabasualto/MJZ/CTP2022/SARDINAAUSTRAL_LAGOS/PRIMER_INFORME/Datos_a_Junio/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01F1DFFA-6341-4943-AAA8-FD37B6104FBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF5E6103-232E-A149-B442-DF644A309673}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="27560" yWindow="3580" windowWidth="23300" windowHeight="22440" xr2:uid="{D73FE552-5237-42B3-AA1B-489DDDA3A168}"/>
+    <workbookView xWindow="6960" yWindow="1580" windowWidth="23300" windowHeight="22440" xr2:uid="{D73FE552-5237-42B3-AA1B-489DDDA3A168}"/>
   </bookViews>
   <sheets>
     <sheet name="XI Region " sheetId="2" r:id="rId1"/>

</xml_diff>